<commit_message>
Anhadir seguridad al servicio y anhadir todos los dispositivos, faltan los id's para el escaner. 15/05/2023
</commit_message>
<xml_diff>
--- a/ServicioREST/Ejemplos.xlsx
+++ b/ServicioREST/Ejemplos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\TFG-MarioIngelmoDiana\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\TFG-MarioIngelmoDiana\ServicioREST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9EC7191-11DE-498F-A9D8-BC9B5B0819F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAE52A7-162A-4A78-AF56-EA5C82E2188E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{83E81272-B4FF-3E48-AF56-765C8A2B6DB7}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{83E81272-B4FF-3E48-AF56-765C8A2B6DB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="61">
   <si>
     <t>Categoría</t>
   </si>
@@ -158,12 +158,6 @@
     <t>Nest Learning Thermostat</t>
   </si>
   <si>
-    <t>Puntuación de seguridad</t>
-  </si>
-  <si>
-    <t>Puntuación de sostenibilidad</t>
-  </si>
-  <si>
     <t>Asistente virtual</t>
   </si>
   <si>
@@ -216,6 +210,15 @@
   </si>
   <si>
     <t>Neato Botvac D7</t>
+  </si>
+  <si>
+    <t>Seguridad</t>
+  </si>
+  <si>
+    <t>Sostenibilidad</t>
+  </si>
+  <si>
+    <t>Precio</t>
   </si>
 </sst>
 </file>
@@ -579,25 +582,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC51AF7D-86C3-6E41-93AF-299C6E973908}">
-  <dimension ref="B6:I31"/>
+  <dimension ref="B5:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="30.796875" customWidth="1"/>
-    <col min="4" max="4" width="31.296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3984375" customWidth="1"/>
+    <col min="3" max="3" width="28.3984375" customWidth="1"/>
+    <col min="4" max="4" width="28.8984375" customWidth="1"/>
+    <col min="5" max="5" width="29.69921875" customWidth="1"/>
+    <col min="6" max="6" width="9.8984375" customWidth="1"/>
     <col min="7" max="7" width="35" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.69921875" customWidth="1"/>
-    <col min="9" max="9" width="11.69921875" customWidth="1"/>
+    <col min="9" max="9" width="12.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:10" s="2" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
@@ -611,7 +615,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>4</v>
@@ -620,36 +624,42 @@
         <v>5</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>70</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>6</v>
       </c>
@@ -659,7 +669,7 @@
       <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>80</v>
       </c>
       <c r="G8" t="s">
@@ -671,31 +681,37 @@
       <c r="I8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J8" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9">
+        <v>43</v>
+      </c>
+      <c r="F9" s="1">
         <v>75</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J9" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>12</v>
       </c>
@@ -705,7 +721,7 @@
       <c r="E10" t="s">
         <v>14</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>70</v>
       </c>
       <c r="G10" t="s">
@@ -717,8 +733,11 @@
       <c r="I10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J10" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>27</v>
       </c>
@@ -728,7 +747,7 @@
       <c r="E11" t="s">
         <v>14</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>55</v>
       </c>
       <c r="G11" t="s">
@@ -740,31 +759,37 @@
       <c r="I11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J11" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12">
+        <v>43</v>
+      </c>
+      <c r="F12" s="1">
         <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J12" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>16</v>
       </c>
@@ -774,7 +799,7 @@
       <c r="E13" t="s">
         <v>14</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>60</v>
       </c>
       <c r="G13" t="s">
@@ -786,8 +811,11 @@
       <c r="I13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J13" s="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>17</v>
       </c>
@@ -797,7 +825,7 @@
       <c r="E14" t="s">
         <v>19</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>40</v>
       </c>
       <c r="G14" t="s">
@@ -809,8 +837,11 @@
       <c r="I14" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J14" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>23</v>
       </c>
@@ -820,7 +851,7 @@
       <c r="E15" t="s">
         <v>25</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>45</v>
       </c>
       <c r="G15" t="s">
@@ -832,34 +863,44 @@
       <c r="I15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J15" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="F16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17">
+        <v>45</v>
+      </c>
+      <c r="F17" s="1">
         <v>80</v>
       </c>
       <c r="G17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J17" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>30</v>
       </c>
@@ -869,7 +910,7 @@
       <c r="E18" t="s">
         <v>32</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <v>85</v>
       </c>
       <c r="G18" t="s">
@@ -881,31 +922,37 @@
       <c r="I18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J18" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19">
+        <v>45</v>
+      </c>
+      <c r="F19" s="1">
         <v>75</v>
       </c>
       <c r="G19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I19" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J19" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>34</v>
       </c>
@@ -915,7 +962,7 @@
       <c r="E20" t="s">
         <v>32</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <v>70</v>
       </c>
       <c r="G20" t="s">
@@ -927,8 +974,11 @@
       <c r="I20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J20" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>35</v>
       </c>
@@ -938,7 +988,7 @@
       <c r="E21" t="s">
         <v>37</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <v>55</v>
       </c>
       <c r="G21" t="s">
@@ -950,34 +1000,44 @@
       <c r="I21" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J21" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="F22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23">
+        <v>43</v>
+      </c>
+      <c r="F23" s="1">
         <v>80</v>
       </c>
       <c r="G23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I23" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J23" s="1">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>39</v>
       </c>
@@ -987,7 +1047,7 @@
       <c r="E24" t="s">
         <v>32</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="1">
         <v>90</v>
       </c>
       <c r="G24" s="1">
@@ -996,126 +1056,152 @@
       <c r="I24" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J24" s="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E25" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25">
+        <v>43</v>
+      </c>
+      <c r="F25" s="1">
         <v>75</v>
       </c>
       <c r="G25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I25" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J25" s="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="F26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E27" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27">
+        <v>43</v>
+      </c>
+      <c r="F27" s="1">
         <v>75</v>
       </c>
       <c r="G27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I27" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J27" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E28" t="s">
-        <v>45</v>
-      </c>
-      <c r="F28">
+        <v>43</v>
+      </c>
+      <c r="F28" s="1">
         <v>70</v>
       </c>
       <c r="G28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I28" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J28" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="F29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
-      </c>
-      <c r="F30">
+        <v>45</v>
+      </c>
+      <c r="F30" s="1">
         <v>85</v>
       </c>
       <c r="G30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I30" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J30" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E31" t="s">
-        <v>47</v>
-      </c>
-      <c r="F31">
+        <v>45</v>
+      </c>
+      <c r="F31" s="1">
         <v>80</v>
       </c>
       <c r="G31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I31" t="s">
         <v>33</v>
+      </c>
+      <c r="J31" s="1">
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>